<commit_message>
recent lab changes: 2025-05-06 04:05:25
</commit_message>
<xml_diff>
--- a/Курс 2/Основы Data Science/Лабораторные/02. Структура и описание данных. Описательные характеристики/gameandgrade.xlsx
+++ b/Курс 2/Основы Data Science/Лабораторные/02. Структура и описание данных. Описательные характеристики/gameandgrade.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/olesteep/Documents/Study/Курс 2/Основы Data Science/Лабораторные/02. Структура и описание данных. Описательные характеристики/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C529DC5-9734-5B4C-809E-56F7F0D76396}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A675A71-78D3-4344-8F3A-8637F93A7C5B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="17360" yWindow="760" windowWidth="17080" windowHeight="21440" activeTab="3" xr2:uid="{94C2AD48-8C41-6147-84AE-58A60A9548F9}"/>
   </bookViews>
@@ -25,8 +25,8 @@
   </definedNames>
   <calcPr calcId="191029"/>
   <pivotCaches>
-    <pivotCache cacheId="12" r:id="rId5"/>
-    <pivotCache cacheId="13" r:id="rId6"/>
+    <pivotCache cacheId="0" r:id="rId5"/>
+    <pivotCache cacheId="1" r:id="rId6"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -262,22 +262,22 @@
     <t>низкое образование - 0, 1, 2</t>
   </si>
   <si>
-    <t>высокое образование - 3, 4, 5</t>
-  </si>
-  <si>
     <t>часто играют - 3, 4, 5</t>
   </si>
   <si>
     <t>мало играют - 0, 1, 2</t>
   </si>
   <si>
-    <t>Двухвыборочный t-тест с одинаковыми дисперсиями (Для матери)</t>
+    <t>п</t>
   </si>
   <si>
-    <t>Двухвыборочный t-тест с одинаковыми дисперсиями (Для отца)</t>
+    <t>высокое образование - 5, 6</t>
   </si>
   <si>
-    <t>п</t>
+    <t>Двухвыборочный t-тест с одинаковыми дисперсиями (для матери)</t>
+  </si>
+  <si>
+    <t>Двухвыборочный t-тест с одинаковыми дисперсиями (для отца)</t>
   </si>
 </sst>
 </file>
@@ -878,12 +878,12 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="21" fillId="35" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="35" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="43">
     <cellStyle name="20% — акцент1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -932,7 +932,7 @@
   </cellStyles>
   <dxfs count="10">
     <dxf>
-      <numFmt numFmtId="1" formatCode="0"/>
+      <numFmt numFmtId="14" formatCode="0.00%"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="164" formatCode="0.000"/>
@@ -944,7 +944,7 @@
       <numFmt numFmtId="164" formatCode="0.000"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="14" formatCode="0.00%"/>
+      <numFmt numFmtId="1" formatCode="0"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="164" formatCode="0.000"/>
@@ -32689,396 +32689,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{7B3673BB-A2E0-9945-A967-74D58F6F93D4}" name="Сводная таблица10" cacheId="12" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Значения" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" multipleFieldFilters="0" chartFormat="12">
-  <location ref="B15:C18" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
-  <pivotFields count="11">
-    <pivotField axis="axisRow" dataField="1" showAll="0">
-      <items count="3">
-        <item x="0"/>
-        <item x="1"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0">
-      <items count="7">
-        <item x="2"/>
-        <item x="4"/>
-        <item x="0"/>
-        <item x="1"/>
-        <item x="5"/>
-        <item x="3"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField dragToRow="0" dragToCol="0" dragToPage="0" showAll="0" defaultSubtotal="0"/>
-  </pivotFields>
-  <rowFields count="1">
-    <field x="0"/>
-  </rowFields>
-  <rowItems count="3">
-    <i>
-      <x/>
-    </i>
-    <i>
-      <x v="1"/>
-    </i>
-    <i t="grand">
-      <x/>
-    </i>
-  </rowItems>
-  <colItems count="1">
-    <i/>
-  </colItems>
-  <dataFields count="1">
-    <dataField name="Количество по полю Sex" fld="0" subtotal="count" baseField="0" baseItem="0" numFmtId="1"/>
-  </dataFields>
-  <formats count="2">
-    <format dxfId="1">
-      <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
-    </format>
-    <format dxfId="0">
-      <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0">
-        <references count="1">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </format>
-  </formats>
-  <chartFormats count="6">
-    <chartFormat chart="3" format="2" series="1">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="1">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="3" format="4">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="2">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-          <reference field="0" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="3" format="5">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="2">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-          <reference field="0" count="1" selected="0">
-            <x v="1"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="11" format="15" series="1">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="1">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="11" format="16">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="2">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-          <reference field="0" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="11" format="17">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="2">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-          <reference field="0" count="1" selected="0">
-            <x v="1"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-  </chartFormats>
-  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
-      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
-    </ext>
-    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
-      <xpdl:pivotTableDefinition16/>
-    </ext>
-  </extLst>
-</pivotTableDefinition>
-</file>
-
-<file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{6A4080B6-CD9C-FB4D-BF75-FB8D52BE33C3}" name="Сводная таблица9" cacheId="13" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Значения" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" multipleFieldFilters="0" chartFormat="24">
-  <location ref="B77:C85" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
-  <pivotFields count="10">
-    <pivotField showAll="0"/>
-    <pivotField dataField="1" showAll="0"/>
-    <pivotField axis="axisRow" showAll="0">
-      <items count="8">
-        <item x="2"/>
-        <item x="4"/>
-        <item x="0"/>
-        <item x="1"/>
-        <item x="5"/>
-        <item x="3"/>
-        <item x="6"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0">
-      <items count="8">
-        <item x="1"/>
-        <item x="0"/>
-        <item x="2"/>
-        <item x="4"/>
-        <item x="5"/>
-        <item x="3"/>
-        <item x="6"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField showAll="0">
-      <items count="13">
-        <item x="0"/>
-        <item x="1"/>
-        <item x="2"/>
-        <item x="3"/>
-        <item x="4"/>
-        <item x="5"/>
-        <item x="6"/>
-        <item x="7"/>
-        <item x="8"/>
-        <item x="9"/>
-        <item x="10"/>
-        <item x="11"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-  </pivotFields>
-  <rowFields count="1">
-    <field x="2"/>
-  </rowFields>
-  <rowItems count="8">
-    <i>
-      <x/>
-    </i>
-    <i>
-      <x v="1"/>
-    </i>
-    <i>
-      <x v="2"/>
-    </i>
-    <i>
-      <x v="3"/>
-    </i>
-    <i>
-      <x v="4"/>
-    </i>
-    <i>
-      <x v="5"/>
-    </i>
-    <i>
-      <x v="6"/>
-    </i>
-    <i t="grand">
-      <x/>
-    </i>
-  </rowItems>
-  <colItems count="1">
-    <i/>
-  </colItems>
-  <dataFields count="1">
-    <dataField name="Количество по полю School Code" fld="1" subtotal="count" showDataAs="percentOfTotal" baseField="0" baseItem="0" numFmtId="10"/>
-  </dataFields>
-  <chartFormats count="2">
-    <chartFormat chart="0" format="1" series="1">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="1">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="23" format="3" series="1">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="1">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-  </chartFormats>
-  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
-      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
-    </ext>
-    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
-      <xpdl:pivotTableDefinition16/>
-    </ext>
-  </extLst>
-</pivotTableDefinition>
-</file>
-
-<file path=xl/pivotTables/pivotTable3.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{547671A9-AF8C-FA4E-857C-C95CFB12C3D8}" name="Сводная таблица14" cacheId="13" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Значения" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" multipleFieldFilters="0" chartFormat="22">
-  <location ref="B90:C97" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
-  <pivotFields count="10">
-    <pivotField showAll="0">
-      <items count="4">
-        <item x="0"/>
-        <item x="1"/>
-        <item x="2"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0">
-      <items count="8">
-        <item x="2"/>
-        <item x="4"/>
-        <item x="0"/>
-        <item x="1"/>
-        <item x="5"/>
-        <item x="3"/>
-        <item x="6"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField axis="axisRow" dataField="1" showAll="0">
-      <items count="7">
-        <item x="1"/>
-        <item x="0"/>
-        <item x="3"/>
-        <item x="2"/>
-        <item x="4"/>
-        <item x="5"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0">
-      <items count="13">
-        <item x="0"/>
-        <item x="1"/>
-        <item x="2"/>
-        <item x="3"/>
-        <item x="4"/>
-        <item x="5"/>
-        <item x="6"/>
-        <item x="7"/>
-        <item x="8"/>
-        <item x="9"/>
-        <item x="10"/>
-        <item x="11"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-  </pivotFields>
-  <rowFields count="1">
-    <field x="7"/>
-  </rowFields>
-  <rowItems count="7">
-    <i>
-      <x/>
-    </i>
-    <i>
-      <x v="1"/>
-    </i>
-    <i>
-      <x v="2"/>
-    </i>
-    <i>
-      <x v="3"/>
-    </i>
-    <i>
-      <x v="4"/>
-    </i>
-    <i>
-      <x v="5"/>
-    </i>
-    <i t="grand">
-      <x/>
-    </i>
-  </rowItems>
-  <colItems count="1">
-    <i/>
-  </colItems>
-  <dataFields count="1">
-    <dataField name="Количество по полю Playing Years" fld="7" subtotal="count" showDataAs="percentOfTotal" baseField="0" baseItem="0" numFmtId="10"/>
-  </dataFields>
-  <chartFormats count="2">
-    <chartFormat chart="0" format="2" series="1">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="1">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="21" format="4" series="1">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="1">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-  </chartFormats>
-  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
-      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
-    </ext>
-    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
-      <xpdl:pivotTableDefinition16/>
-    </ext>
-  </extLst>
-</pivotTableDefinition>
-</file>
-
-<file path=xl/pivotTables/pivotTable4.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{74925334-BBB6-8E4D-A8C4-1418A3312DE5}" name="Сводная таблица13" cacheId="12" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Значения" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" multipleFieldFilters="0" chartFormat="42">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{74925334-BBB6-8E4D-A8C4-1418A3312DE5}" name="Сводная таблица13" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Значения" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" multipleFieldFilters="0" chartFormat="42">
   <location ref="B25:C33" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="11">
     <pivotField showAll="0"/>
@@ -33150,10 +32761,10 @@
     <dataField name="Количество по полю Mother Education" fld="4" subtotal="count" showDataAs="percentOfTotal" baseField="0" baseItem="0" numFmtId="10"/>
   </dataFields>
   <formats count="2">
-    <format dxfId="3">
+    <format dxfId="1">
       <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
     </format>
-    <format dxfId="2">
+    <format dxfId="0">
       <pivotArea outline="0" fieldPosition="0">
         <references count="1">
           <reference field="4294967294" count="1">
@@ -33195,8 +32806,8 @@
 </pivotTableDefinition>
 </file>
 
-<file path=xl/pivotTables/pivotTable5.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{C4055949-EA7B-2D47-839F-58ABF0D24DC6}" name="Сводная таблица8" cacheId="12" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Значения" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" multipleFieldFilters="0" chartFormat="47">
+<file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{C4055949-EA7B-2D47-839F-58ABF0D24DC6}" name="Сводная таблица8" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Значения" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" multipleFieldFilters="0" chartFormat="47">
   <location ref="B51:C58" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="11">
     <pivotField showAll="0"/>
@@ -33275,10 +32886,10 @@
     <dataField name="Количество по полю Playing Hours" fld="8" subtotal="count" showDataAs="percentOfTotal" baseField="0" baseItem="0" numFmtId="10"/>
   </dataFields>
   <formats count="2">
-    <format dxfId="5">
+    <format dxfId="3">
       <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
     </format>
-    <format dxfId="4">
+    <format dxfId="2">
       <pivotArea outline="0" fieldPosition="0">
         <references count="1">
           <reference field="4294967294" count="1">
@@ -33320,8 +32931,8 @@
 </pivotTableDefinition>
 </file>
 
-<file path=xl/pivotTables/pivotTable6.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{20128A8E-8F8D-1F4B-B63D-08C20AED7F0D}" name="Сводная таблица12" cacheId="13" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Значения" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="10">
+<file path=xl/pivotTables/pivotTable3.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{20128A8E-8F8D-1F4B-B63D-08C20AED7F0D}" name="Сводная таблица12" cacheId="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Значения" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="10">
   <location ref="B101:C112" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="10">
     <pivotField showAll="0"/>
@@ -33445,8 +33056,274 @@
 </pivotTableDefinition>
 </file>
 
-<file path=xl/pivotTables/pivotTable7.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{AB5542E4-160E-E945-9B5A-ED309DB05DB7}" name="Сводная таблица7" cacheId="12" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Значения" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" multipleFieldFilters="0" chartFormat="25">
+<file path=xl/pivotTables/pivotTable4.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{7B3673BB-A2E0-9945-A967-74D58F6F93D4}" name="Сводная таблица10" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Значения" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" multipleFieldFilters="0" chartFormat="12">
+  <location ref="B15:C18" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
+  <pivotFields count="11">
+    <pivotField axis="axisRow" dataField="1" showAll="0">
+      <items count="3">
+        <item x="0"/>
+        <item x="1"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0">
+      <items count="7">
+        <item x="2"/>
+        <item x="4"/>
+        <item x="0"/>
+        <item x="1"/>
+        <item x="5"/>
+        <item x="3"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField dragToRow="0" dragToCol="0" dragToPage="0" showAll="0" defaultSubtotal="0"/>
+  </pivotFields>
+  <rowFields count="1">
+    <field x="0"/>
+  </rowFields>
+  <rowItems count="3">
+    <i>
+      <x/>
+    </i>
+    <i>
+      <x v="1"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </rowItems>
+  <colItems count="1">
+    <i/>
+  </colItems>
+  <dataFields count="1">
+    <dataField name="Количество по полю Sex" fld="0" subtotal="count" baseField="0" baseItem="0" numFmtId="1"/>
+  </dataFields>
+  <formats count="2">
+    <format dxfId="5">
+      <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
+    </format>
+    <format dxfId="4">
+      <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+  </formats>
+  <chartFormats count="6">
+    <chartFormat chart="3" format="2" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="3" format="4">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="0" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="3" format="5">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="0" count="1" selected="0">
+            <x v="1"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="11" format="15" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="11" format="16">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="0" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="11" format="17">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="0" count="1" selected="0">
+            <x v="1"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+  </chartFormats>
+  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
+      <xpdl:pivotTableDefinition16/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
+<file path=xl/pivotTables/pivotTable5.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{6A4080B6-CD9C-FB4D-BF75-FB8D52BE33C3}" name="Сводная таблица9" cacheId="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Значения" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" multipleFieldFilters="0" chartFormat="24">
+  <location ref="B77:C85" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
+  <pivotFields count="10">
+    <pivotField showAll="0"/>
+    <pivotField dataField="1" showAll="0"/>
+    <pivotField axis="axisRow" showAll="0">
+      <items count="8">
+        <item x="2"/>
+        <item x="4"/>
+        <item x="0"/>
+        <item x="1"/>
+        <item x="5"/>
+        <item x="3"/>
+        <item x="6"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0">
+      <items count="8">
+        <item x="1"/>
+        <item x="0"/>
+        <item x="2"/>
+        <item x="4"/>
+        <item x="5"/>
+        <item x="3"/>
+        <item x="6"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0">
+      <items count="13">
+        <item x="0"/>
+        <item x="1"/>
+        <item x="2"/>
+        <item x="3"/>
+        <item x="4"/>
+        <item x="5"/>
+        <item x="6"/>
+        <item x="7"/>
+        <item x="8"/>
+        <item x="9"/>
+        <item x="10"/>
+        <item x="11"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+  </pivotFields>
+  <rowFields count="1">
+    <field x="2"/>
+  </rowFields>
+  <rowItems count="8">
+    <i>
+      <x/>
+    </i>
+    <i>
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="2"/>
+    </i>
+    <i>
+      <x v="3"/>
+    </i>
+    <i>
+      <x v="4"/>
+    </i>
+    <i>
+      <x v="5"/>
+    </i>
+    <i>
+      <x v="6"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </rowItems>
+  <colItems count="1">
+    <i/>
+  </colItems>
+  <dataFields count="1">
+    <dataField name="Количество по полю School Code" fld="1" subtotal="count" showDataAs="percentOfTotal" baseField="0" baseItem="0" numFmtId="10"/>
+  </dataFields>
+  <chartFormats count="2">
+    <chartFormat chart="0" format="1" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="23" format="3" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+  </chartFormats>
+  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
+      <xpdl:pivotTableDefinition16/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
+<file path=xl/pivotTables/pivotTable6.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{AB5542E4-160E-E945-9B5A-ED309DB05DB7}" name="Сводная таблица7" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Значения" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" multipleFieldFilters="0" chartFormat="25">
   <location ref="B64:C70" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="11">
     <pivotField showAll="0"/>
@@ -33566,8 +33443,131 @@
 </pivotTableDefinition>
 </file>
 
+<file path=xl/pivotTables/pivotTable7.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{547671A9-AF8C-FA4E-857C-C95CFB12C3D8}" name="Сводная таблица14" cacheId="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Значения" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" multipleFieldFilters="0" chartFormat="22">
+  <location ref="B90:C97" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
+  <pivotFields count="10">
+    <pivotField showAll="0">
+      <items count="4">
+        <item x="0"/>
+        <item x="1"/>
+        <item x="2"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0">
+      <items count="8">
+        <item x="2"/>
+        <item x="4"/>
+        <item x="0"/>
+        <item x="1"/>
+        <item x="5"/>
+        <item x="3"/>
+        <item x="6"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField axis="axisRow" dataField="1" showAll="0">
+      <items count="7">
+        <item x="1"/>
+        <item x="0"/>
+        <item x="3"/>
+        <item x="2"/>
+        <item x="4"/>
+        <item x="5"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0">
+      <items count="13">
+        <item x="0"/>
+        <item x="1"/>
+        <item x="2"/>
+        <item x="3"/>
+        <item x="4"/>
+        <item x="5"/>
+        <item x="6"/>
+        <item x="7"/>
+        <item x="8"/>
+        <item x="9"/>
+        <item x="10"/>
+        <item x="11"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+  </pivotFields>
+  <rowFields count="1">
+    <field x="7"/>
+  </rowFields>
+  <rowItems count="7">
+    <i>
+      <x/>
+    </i>
+    <i>
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="2"/>
+    </i>
+    <i>
+      <x v="3"/>
+    </i>
+    <i>
+      <x v="4"/>
+    </i>
+    <i>
+      <x v="5"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </rowItems>
+  <colItems count="1">
+    <i/>
+  </colItems>
+  <dataFields count="1">
+    <dataField name="Количество по полю Playing Years" fld="7" subtotal="count" showDataAs="percentOfTotal" baseField="0" baseItem="0" numFmtId="10"/>
+  </dataFields>
+  <chartFormats count="2">
+    <chartFormat chart="0" format="2" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="21" format="4" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+  </chartFormats>
+  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
+      <xpdl:pivotTableDefinition16/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
 <file path=xl/pivotTables/pivotTable8.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{96E7D066-6BCD-C74A-A456-629E58FD8256}" name="Сводная таблица11" cacheId="12" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Значения" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" multipleFieldFilters="0" chartFormat="23">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{96E7D066-6BCD-C74A-A456-629E58FD8256}" name="Сводная таблица11" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Значения" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" multipleFieldFilters="0" chartFormat="23">
   <location ref="B38:C46" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="11">
     <pivotField showAll="0"/>
@@ -33987,8 +33987,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F30EAD57-2722-2640-9045-129DE337E71B}">
   <dimension ref="A1:U773"/>
   <sheetViews>
-    <sheetView topLeftCell="A394" zoomScale="75" zoomScaleNormal="81" workbookViewId="0">
-      <selection activeCell="J415" sqref="A1:J415"/>
+    <sheetView topLeftCell="A2" zoomScale="75" zoomScaleNormal="81" workbookViewId="0">
+      <selection activeCell="E2" sqref="A2:J771"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -58711,41 +58711,41 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{75069B8F-3AE3-DD4F-B9E5-3A5847B7AA82}">
   <dimension ref="A1:J357"/>
   <sheetViews>
-    <sheetView topLeftCell="A291" zoomScale="75" workbookViewId="0">
-      <selection activeCell="J16" sqref="J16"/>
+    <sheetView topLeftCell="A313" zoomScale="75" workbookViewId="0">
+      <selection activeCell="J2" sqref="J2:J68"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1" s="23" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="23" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="23" t="s">
-        <v>3</v>
-      </c>
-      <c r="D1" s="23" t="s">
-        <v>5</v>
-      </c>
-      <c r="E1" s="23" t="s">
+      <c r="A1" s="20" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="20" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="20" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" s="20" t="s">
+        <v>5</v>
+      </c>
+      <c r="E1" s="20" t="s">
         <v>8</v>
       </c>
-      <c r="F1" s="23" t="s">
+      <c r="F1" s="20" t="s">
         <v>7</v>
       </c>
-      <c r="G1" s="23" t="s">
+      <c r="G1" s="20" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="23" t="s">
-        <v>2</v>
-      </c>
-      <c r="I1" s="23" t="s">
-        <v>4</v>
-      </c>
-      <c r="J1" s="23" t="s">
+      <c r="H1" s="20" t="s">
+        <v>2</v>
+      </c>
+      <c r="I1" s="20" t="s">
+        <v>4</v>
+      </c>
+      <c r="J1" s="20" t="s">
         <v>9</v>
       </c>
     </row>
@@ -70155,7 +70155,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0A424681-3FE9-694E-A0B1-02F687C4B387}">
   <dimension ref="B2:E112"/>
   <sheetViews>
-    <sheetView topLeftCell="C76" zoomScale="125" workbookViewId="0">
+    <sheetView topLeftCell="B21" zoomScale="125" workbookViewId="0">
       <selection activeCell="C108" sqref="C102:C108"/>
     </sheetView>
   </sheetViews>
@@ -70863,8 +70863,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B8AF8D23-ABA4-1A44-B54C-CBEFB7E9A58E}">
   <dimension ref="A2:O772"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="82" zoomScaleNormal="134" workbookViewId="0">
-      <selection activeCell="F21" sqref="F21"/>
+    <sheetView tabSelected="1" zoomScale="82" zoomScaleNormal="82" workbookViewId="0">
+      <selection activeCell="F18" sqref="F18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -70892,16 +70892,16 @@
         <v>64</v>
       </c>
       <c r="C4" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
       <c r="O4" s="17"/>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.2">
       <c r="B5" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C5" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="O5" s="17"/>
     </row>
@@ -70910,7 +70910,7 @@
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="O7" s="17"/>
     </row>
@@ -70918,129 +70918,129 @@
       <c r="O8" s="17"/>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A9" s="22"/>
-      <c r="B9" s="22" t="s">
+      <c r="A9" s="23"/>
+      <c r="B9" s="23" t="s">
         <v>42</v>
       </c>
-      <c r="C9" s="22" t="s">
+      <c r="C9" s="23" t="s">
         <v>43</v>
       </c>
       <c r="O9" s="17"/>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A10" s="20" t="s">
+      <c r="A10" s="21" t="s">
         <v>44</v>
       </c>
-      <c r="B10" s="20">
-        <v>1.8160919540229885</v>
-      </c>
-      <c r="C10" s="20">
-        <v>3.9516728624535316</v>
+      <c r="B10" s="21">
+        <v>71.281954022988501</v>
+      </c>
+      <c r="C10" s="21">
+        <v>87.568181818181813</v>
       </c>
       <c r="O10" s="17"/>
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A11" s="20" t="s">
+      <c r="A11" s="21" t="s">
         <v>45</v>
       </c>
-      <c r="B11" s="20">
-        <v>0.15183106121357898</v>
-      </c>
-      <c r="C11" s="20">
-        <v>0.73273040004438816</v>
+      <c r="B11" s="21">
+        <v>254.01051823041999</v>
+      </c>
+      <c r="C11" s="21">
+        <v>275.52989510489505</v>
       </c>
       <c r="O11" s="17"/>
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A12" s="20" t="s">
+      <c r="A12" s="21" t="s">
         <v>46</v>
       </c>
-      <c r="B12" s="20">
+      <c r="B12" s="21">
         <v>87</v>
       </c>
-      <c r="C12" s="20">
-        <v>269</v>
+      <c r="C12" s="21">
+        <v>66</v>
       </c>
       <c r="O12" s="17"/>
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A13" s="20" t="s">
+      <c r="A13" s="21" t="s">
         <v>47</v>
       </c>
-      <c r="B13" s="20">
-        <v>0.59160796179735542</v>
-      </c>
-      <c r="C13" s="20"/>
+      <c r="B13" s="21">
+        <v>263.27382615651851</v>
+      </c>
+      <c r="C13" s="21"/>
       <c r="O13" s="17"/>
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A14" s="20" t="s">
+      <c r="A14" s="21" t="s">
         <v>48</v>
       </c>
-      <c r="B14" s="20">
-        <v>0</v>
-      </c>
-      <c r="C14" s="20"/>
+      <c r="B14" s="21">
+        <v>0</v>
+      </c>
+      <c r="C14" s="21"/>
       <c r="O14" s="17"/>
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A15" s="20" t="s">
+      <c r="A15" s="21" t="s">
         <v>49</v>
       </c>
-      <c r="B15" s="20">
-        <v>354</v>
-      </c>
-      <c r="C15" s="20"/>
+      <c r="B15" s="21">
+        <v>151</v>
+      </c>
+      <c r="C15" s="21"/>
       <c r="O15" s="17"/>
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A16" s="20" t="s">
+      <c r="A16" s="21" t="s">
         <v>50</v>
       </c>
-      <c r="B16" s="20">
-        <v>-22.511777725256401</v>
-      </c>
-      <c r="C16" s="20"/>
+      <c r="B16" s="21">
+        <v>-6.1489723632650639</v>
+      </c>
+      <c r="C16" s="21"/>
       <c r="O16" s="17"/>
     </row>
     <row r="17" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A17" s="20" t="s">
+      <c r="A17" s="21" t="s">
         <v>51</v>
       </c>
-      <c r="B17" s="20">
-        <v>1.3738570005292101E-70</v>
-      </c>
-      <c r="C17" s="20"/>
+      <c r="B17" s="21">
+        <v>3.327541620635482E-9</v>
+      </c>
+      <c r="C17" s="21"/>
       <c r="O17" s="17"/>
     </row>
     <row r="18" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A18" s="20" t="s">
+      <c r="A18" s="21" t="s">
         <v>52</v>
       </c>
-      <c r="B18" s="20">
-        <v>1.6491694147322193</v>
-      </c>
-      <c r="C18" s="20"/>
+      <c r="B18" s="21">
+        <v>1.6550073865802402</v>
+      </c>
+      <c r="C18" s="21"/>
       <c r="O18" s="17"/>
     </row>
     <row r="19" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A19" s="20" t="s">
+      <c r="A19" s="21" t="s">
         <v>53</v>
       </c>
-      <c r="B19" s="20">
-        <v>2.7477140010584202E-70</v>
-      </c>
-      <c r="C19" s="20"/>
+      <c r="B19" s="21">
+        <v>6.6550832412709639E-9</v>
+      </c>
+      <c r="C19" s="21"/>
       <c r="O19" s="17"/>
     </row>
     <row r="20" spans="1:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="21" t="s">
+      <c r="A20" s="22" t="s">
         <v>54</v>
       </c>
-      <c r="B20" s="21">
-        <v>1.9666878964647558</v>
-      </c>
-      <c r="C20" s="21"/>
+      <c r="B20" s="22">
+        <v>1.9757989238179368</v>
+      </c>
+      <c r="C20" s="22"/>
       <c r="O20" s="17"/>
     </row>
     <row r="21" spans="1:15" x14ac:dyDescent="0.2">
@@ -71050,7 +71050,7 @@
     </row>
     <row r="22" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="O22" s="17"/>
     </row>
@@ -71058,132 +71058,132 @@
       <c r="O23" s="17"/>
     </row>
     <row r="24" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A24" s="22"/>
-      <c r="B24" s="22" t="s">
+      <c r="A24" s="23"/>
+      <c r="B24" s="23" t="s">
         <v>42</v>
       </c>
-      <c r="C24" s="22" t="s">
+      <c r="C24" s="23" t="s">
         <v>43</v>
       </c>
       <c r="O24" s="17"/>
     </row>
     <row r="25" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A25" s="20" t="s">
+      <c r="A25" s="21" t="s">
         <v>44</v>
       </c>
-      <c r="B25" s="20">
-        <v>1.8955223880597014</v>
-      </c>
-      <c r="C25" s="20">
-        <v>4.1141868512110724</v>
+      <c r="B25" s="21">
+        <v>72.546716417910446</v>
+      </c>
+      <c r="C25" s="21">
+        <v>84.955555555555549</v>
       </c>
       <c r="O25" s="17"/>
     </row>
     <row r="26" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A26" s="20" t="s">
+      <c r="A26" s="21" t="s">
         <v>45</v>
       </c>
-      <c r="B26" s="20">
-        <v>0.15558570782451397</v>
-      </c>
-      <c r="C26" s="20">
-        <v>0.81677720107650964</v>
+      <c r="B26" s="21">
+        <v>263.24067693351412</v>
+      </c>
+      <c r="C26" s="21">
+        <v>275.37440699126097</v>
       </c>
       <c r="O26" s="17"/>
     </row>
     <row r="27" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A27" s="20" t="s">
+      <c r="A27" s="21" t="s">
         <v>46</v>
       </c>
-      <c r="B27" s="20">
+      <c r="B27" s="21">
         <v>67</v>
       </c>
-      <c r="C27" s="20">
-        <v>289</v>
+      <c r="C27" s="21">
+        <v>90</v>
       </c>
       <c r="O27" s="17"/>
     </row>
     <row r="28" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A28" s="20" t="s">
+      <c r="A28" s="21" t="s">
         <v>47</v>
       </c>
-      <c r="B28" s="20">
-        <v>0.69350421080918834</v>
-      </c>
-      <c r="C28" s="20"/>
+      <c r="B28" s="21">
+        <v>270.20778645054293</v>
+      </c>
+      <c r="C28" s="21"/>
       <c r="O28" s="17"/>
     </row>
     <row r="29" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A29" s="20" t="s">
+      <c r="A29" s="21" t="s">
         <v>48</v>
       </c>
-      <c r="B29" s="20">
-        <v>0</v>
-      </c>
-      <c r="C29" s="20"/>
+      <c r="B29" s="21">
+        <v>0</v>
+      </c>
+      <c r="C29" s="21"/>
       <c r="O29" s="17"/>
     </row>
     <row r="30" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A30" s="20" t="s">
+      <c r="A30" s="21" t="s">
         <v>49</v>
       </c>
-      <c r="B30" s="20">
-        <v>354</v>
-      </c>
-      <c r="C30" s="20"/>
+      <c r="B30" s="21">
+        <v>155</v>
+      </c>
+      <c r="C30" s="21"/>
       <c r="O30" s="17"/>
     </row>
     <row r="31" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A31" s="20" t="s">
+      <c r="A31" s="21" t="s">
         <v>50</v>
       </c>
-      <c r="B31" s="20">
-        <v>-19.648454694398335</v>
-      </c>
-      <c r="C31" s="20"/>
+      <c r="B31" s="21">
+        <v>-4.6783321738193848</v>
+      </c>
+      <c r="C31" s="21"/>
       <c r="O31" s="17"/>
     </row>
     <row r="32" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A32" s="20" t="s">
+      <c r="A32" s="21" t="s">
         <v>51</v>
       </c>
-      <c r="B32" s="20">
-        <v>6.0178623308766174E-59</v>
-      </c>
-      <c r="C32" s="20"/>
+      <c r="B32" s="21">
+        <v>3.1284861316859455E-6</v>
+      </c>
+      <c r="C32" s="21"/>
       <c r="O32" s="17"/>
     </row>
     <row r="33" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A33" s="20" t="s">
+      <c r="A33" s="21" t="s">
         <v>52</v>
       </c>
-      <c r="B33" s="20">
-        <v>1.6491694147322193</v>
-      </c>
-      <c r="C33" s="20"/>
+      <c r="B33" s="21">
+        <v>1.6547437739197817</v>
+      </c>
+      <c r="C33" s="21"/>
       <c r="O33" s="17"/>
     </row>
     <row r="34" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A34" s="20" t="s">
+      <c r="A34" s="21" t="s">
         <v>53</v>
       </c>
-      <c r="B34" s="20">
-        <v>1.2035724661753235E-58</v>
-      </c>
-      <c r="C34" s="20"/>
+      <c r="B34" s="21">
+        <v>6.2569722633718909E-6</v>
+      </c>
+      <c r="C34" s="21"/>
       <c r="E34" s="18"/>
       <c r="F34" s="18"/>
       <c r="G34" s="18"/>
       <c r="O34" s="17"/>
     </row>
     <row r="35" spans="1:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="21" t="s">
+      <c r="A35" s="22" t="s">
         <v>54</v>
       </c>
-      <c r="B35" s="21">
-        <v>1.9666878964647558</v>
-      </c>
-      <c r="C35" s="21"/>
+      <c r="B35" s="22">
+        <v>1.9753871310551163</v>
+      </c>
+      <c r="C35" s="22"/>
       <c r="O35" s="17"/>
     </row>
     <row r="36" spans="1:15" x14ac:dyDescent="0.2">
@@ -71389,7 +71389,7 @@
         <v>2.422857142857143</v>
       </c>
       <c r="D63" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="O63" s="17"/>
     </row>

</xml_diff>